<commit_message>
logisim project file added & control signals update 1
</commit_message>
<xml_diff>
--- a/control_codes.xlsx
+++ b/control_codes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,15 +13,165 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+  <si>
+    <t>Opcode</t>
+  </si>
+  <si>
+    <t>Instruction ID</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>ori</t>
+  </si>
+  <si>
+    <t>nor</t>
+  </si>
+  <si>
+    <t>andi</t>
+  </si>
+  <si>
+    <t>sub</t>
+  </si>
+  <si>
+    <t>sll</t>
+  </si>
+  <si>
+    <t>srl</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>bneq</t>
+  </si>
+  <si>
+    <t>subi</t>
+  </si>
+  <si>
+    <t>beq</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>addi</t>
+  </si>
+  <si>
+    <t>lw</t>
+  </si>
+  <si>
+    <t>RegDst</t>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>MemRead</t>
+  </si>
+  <si>
+    <t>MemtoReg</t>
+  </si>
+  <si>
+    <t>ALUOp</t>
+  </si>
+  <si>
+    <t>MemWrite</t>
+  </si>
+  <si>
+    <t>ALUSrc</t>
+  </si>
+  <si>
+    <t>RegWrite</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -44,14 +194,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +309,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +517,616 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="3" width="9.140625" style="2"/>
+    <col min="4" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="9.140625" style="5"/>
+    <col min="10" max="12" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>101</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>110</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>111</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>1001</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>1010</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>1011</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>1100</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>1101</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>1110</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>1111</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Control & Data Memory added
</commit_message>
<xml_diff>
--- a/control_codes.xlsx
+++ b/control_codes.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="control_codes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Opcode</t>
   </si>
@@ -149,14 +149,45 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>ControlBin</t>
+  </si>
+  <si>
+    <t>ControlHex</t>
+  </si>
+  <si>
+    <t>0d00</t>
+  </si>
+  <si>
+    <t>c00</t>
+  </si>
+  <si>
+    <t>8c1</t>
+  </si>
+  <si>
+    <t>cc0</t>
+  </si>
+  <si>
+    <t>c80</t>
+  </si>
+  <si>
+    <t>c18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0000"/>
+    <numFmt numFmtId="166" formatCode="0000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -208,11 +239,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,10 +568,13 @@
     <col min="2" max="3" width="9.140625" style="2"/>
     <col min="4" max="8" width="9.140625" style="4"/>
     <col min="9" max="9" width="9.140625" style="5"/>
-    <col min="10" max="12" width="9.140625" style="4"/>
+    <col min="10" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="19.140625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="5"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -543,7 +584,7 @@
       <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -570,8 +611,17 @@
       <c r="L1" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -596,6 +646,9 @@
       <c r="H2" s="4">
         <v>0</v>
       </c>
+      <c r="I2" s="5">
+        <v>10</v>
+      </c>
       <c r="J2" s="4">
         <v>0</v>
       </c>
@@ -605,8 +658,18 @@
       <c r="L2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="8">
+        <v>100010000001</v>
+      </c>
+      <c r="O2" s="5">
+        <v>881</v>
+      </c>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -631,6 +694,9 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
       <c r="J3" s="4">
         <v>0</v>
       </c>
@@ -640,8 +706,17 @@
       <c r="L3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="8">
+        <v>100000000001</v>
+      </c>
+      <c r="O3" s="5">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>10</v>
       </c>
@@ -666,6 +741,9 @@
       <c r="H4" s="4">
         <v>0</v>
       </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
       <c r="J4" s="4">
         <v>0</v>
       </c>
@@ -675,8 +753,17 @@
       <c r="L4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="8">
+        <v>110100000000</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>11</v>
       </c>
@@ -701,6 +788,9 @@
       <c r="H5" s="4">
         <v>0</v>
       </c>
+      <c r="I5" s="5">
+        <v>1100</v>
+      </c>
       <c r="J5" s="4">
         <v>0</v>
       </c>
@@ -710,8 +800,17 @@
       <c r="L5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="8">
+        <v>100001100001</v>
+      </c>
+      <c r="O5" s="5">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>100</v>
       </c>
@@ -736,6 +835,9 @@
       <c r="H6" s="4">
         <v>0</v>
       </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
       <c r="J6" s="4">
         <v>0</v>
       </c>
@@ -745,8 +847,17 @@
       <c r="L6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="8">
+        <v>110000000000</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>101</v>
       </c>
@@ -771,6 +882,9 @@
       <c r="H7" s="4">
         <v>0</v>
       </c>
+      <c r="I7" s="5">
+        <v>110</v>
+      </c>
       <c r="J7" s="4">
         <v>0</v>
       </c>
@@ -780,8 +894,17 @@
       <c r="L7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>100011000001</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>110</v>
       </c>
@@ -806,14 +929,29 @@
       <c r="H8" s="4">
         <v>0</v>
       </c>
+      <c r="I8" s="5">
+        <v>1000</v>
+      </c>
       <c r="J8" s="4">
         <v>0</v>
       </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
       <c r="L8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="8">
+        <v>1100000100001</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>111</v>
       </c>
@@ -838,14 +976,29 @@
       <c r="H9" s="4">
         <v>0</v>
       </c>
+      <c r="I9" s="5">
+        <v>1001</v>
+      </c>
       <c r="J9" s="4">
         <v>0</v>
       </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
       <c r="L9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="8">
+        <v>1100100100001</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1000</v>
       </c>
@@ -855,8 +1008,8 @@
       <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4">
-        <v>0</v>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -870,6 +1023,9 @@
       <c r="H10" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="I10" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="J10" s="4">
         <v>1</v>
       </c>
@@ -879,8 +1035,17 @@
       <c r="L10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="8">
+        <v>11000000000</v>
+      </c>
+      <c r="O10" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1001</v>
       </c>
@@ -890,8 +1055,8 @@
       <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4">
-        <v>0</v>
+      <c r="D11" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>
@@ -905,6 +1070,9 @@
       <c r="H11" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="I11" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="J11" s="4">
         <v>0</v>
       </c>
@@ -914,8 +1082,17 @@
       <c r="L11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="8">
+        <v>100</v>
+      </c>
+      <c r="O11" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1010</v>
       </c>
@@ -940,6 +1117,9 @@
       <c r="H12" s="4">
         <v>0</v>
       </c>
+      <c r="I12" s="5">
+        <v>110</v>
+      </c>
       <c r="J12" s="4">
         <v>0</v>
       </c>
@@ -949,8 +1129,17 @@
       <c r="L12" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="8">
+        <v>110011000000</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1011</v>
       </c>
@@ -960,8 +1149,8 @@
       <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
+      <c r="D13" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -975,6 +1164,9 @@
       <c r="H13" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="I13" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="J13" s="4">
         <v>0</v>
       </c>
@@ -984,8 +1176,17 @@
       <c r="L13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="8">
+        <v>100</v>
+      </c>
+      <c r="O13" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1100</v>
       </c>
@@ -995,8 +1196,8 @@
       <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="4">
-        <v>0</v>
+      <c r="D14" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
@@ -1010,6 +1211,9 @@
       <c r="H14" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="I14" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="J14" s="4">
         <v>0</v>
       </c>
@@ -1019,8 +1223,17 @@
       <c r="L14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="8">
+        <v>10</v>
+      </c>
+      <c r="O14" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>1101</v>
       </c>
@@ -1045,6 +1258,9 @@
       <c r="H15" s="4">
         <v>0</v>
       </c>
+      <c r="I15" s="5">
+        <v>10</v>
+      </c>
       <c r="J15" s="4">
         <v>0</v>
       </c>
@@ -1054,8 +1270,17 @@
       <c r="L15" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="8">
+        <v>110010000000</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1110</v>
       </c>
@@ -1080,6 +1305,9 @@
       <c r="H16" s="4">
         <v>1</v>
       </c>
+      <c r="I16" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="J16" s="4">
         <v>0</v>
       </c>
@@ -1089,8 +1317,17 @@
       <c r="L16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="8">
+        <v>110000011000</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1111</v>
       </c>
@@ -1115,6 +1352,9 @@
       <c r="H17" s="4">
         <v>0</v>
       </c>
+      <c r="I17" s="5">
+        <v>1</v>
+      </c>
       <c r="J17" s="4">
         <v>0</v>
       </c>
@@ -1123,6 +1363,15 @@
       </c>
       <c r="L17" s="4">
         <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="8">
+        <v>100100000001</v>
+      </c>
+      <c r="O17" s="5">
+        <v>901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working Version 4, sll, srl and j instructions fixed in assembler
</commit_message>
<xml_diff>
--- a/control_codes.xlsx
+++ b/control_codes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="control_codes" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Opcode</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>002c</t>
+  </si>
+  <si>
+    <t>Bneq</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,23 +224,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -546,71 +548,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="3" width="9.140625" style="2"/>
-    <col min="4" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="9.140625" style="5"/>
-    <col min="10" max="13" width="9.140625" style="4"/>
-    <col min="14" max="14" width="19.140625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="5"/>
-    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="9.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="10" style="3" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="20.42578125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="11" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -619,46 +628,48 @@
       <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
         <v>10</v>
       </c>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>1</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="8">
-        <v>1000000100010</v>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
       </c>
       <c r="O2" s="5">
+        <v>10000001000100</v>
+      </c>
+      <c r="P2" s="4">
         <v>1022</v>
       </c>
-      <c r="P2" s="8"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -667,45 +678,48 @@
       <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
         <v>0</v>
       </c>
       <c r="J3" s="4">
         <v>0</v>
       </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
-        <v>1</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>1000000000010</v>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
       </c>
       <c r="O3" s="5">
+        <v>10000000000100</v>
+      </c>
+      <c r="P3" s="4">
         <v>1002</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -714,45 +728,48 @@
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1</v>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
       </c>
       <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="8">
-        <v>10110</v>
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
       </c>
       <c r="O4" s="5">
+        <v>101100</v>
+      </c>
+      <c r="P4" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -761,45 +778,48 @@
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
         <v>1100</v>
       </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="8">
-        <v>1000011000010</v>
-      </c>
-      <c r="O5" s="5" t="s">
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>10000110000100</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>100</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -808,45 +828,48 @@
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
         <v>0</v>
       </c>
       <c r="J6" s="4">
         <v>0</v>
       </c>
-      <c r="K6" s="4">
-        <v>1</v>
-      </c>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-      <c r="N6" s="8">
-        <v>110</v>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
       </c>
       <c r="O6" s="5">
+        <v>1100</v>
+      </c>
+      <c r="P6" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>101</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -855,45 +878,48 @@
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
         <v>110</v>
       </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>1</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="8">
-        <v>1000001100010</v>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
       </c>
       <c r="O7" s="5">
+        <v>10000011000100</v>
+      </c>
+      <c r="P7" s="4">
         <v>1062</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>110</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -902,45 +928,48 @@
       <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
         <v>1000</v>
       </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>1</v>
-      </c>
-      <c r="M8" s="4">
-        <v>1</v>
-      </c>
-      <c r="N8" s="8">
-        <v>1000010000011</v>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1</v>
       </c>
       <c r="O8" s="5">
+        <v>10000100000110</v>
+      </c>
+      <c r="P8" s="4">
         <v>1083</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>111</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -949,45 +978,48 @@
       <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
         <v>1001</v>
       </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>1</v>
-      </c>
-      <c r="M9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" s="8">
-        <v>1000010010011</v>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1</v>
       </c>
       <c r="O9" s="5">
+        <v>10000100100110</v>
+      </c>
+      <c r="P9" s="4">
         <v>1093</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>1000</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -996,45 +1028,48 @@
       <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="4">
         <v>10</v>
       </c>
-      <c r="J10" s="4">
-        <v>1</v>
-      </c>
-      <c r="K10" s="4">
-        <v>1</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-      <c r="N10" s="8">
-        <v>101100</v>
-      </c>
-      <c r="O10" s="5" t="s">
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1011000</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>1001</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1043,45 +1078,48 @@
       <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-      <c r="N11" s="8">
-        <v>10000000000</v>
+        <v>110</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
       </c>
       <c r="O11" s="5">
-        <v>400</v>
+        <v>10000001100000</v>
+      </c>
+      <c r="P11" s="4">
+        <v>2060</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>1010</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1090,45 +1128,48 @@
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
         <v>110</v>
       </c>
-      <c r="J12" s="4">
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <v>1</v>
-      </c>
-      <c r="L12" s="4">
-        <v>1</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0</v>
-      </c>
-      <c r="N12" s="8">
-        <v>1100110</v>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
       </c>
       <c r="O12" s="5">
+        <v>11001100</v>
+      </c>
+      <c r="P12" s="4">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>1011</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1137,45 +1178,48 @@
       <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="J13" s="4">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-      <c r="N13" s="8">
-        <v>10000000000</v>
+        <v>110</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
       </c>
       <c r="O13" s="5">
-        <v>400</v>
+        <v>10001100000</v>
+      </c>
+      <c r="P13" s="4">
+        <v>460</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>1100</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1184,45 +1228,48 @@
       <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-      <c r="N14" s="8">
-        <v>100000000000</v>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
       </c>
       <c r="O14" s="5">
+        <v>1000000000000</v>
+      </c>
+      <c r="P14" s="4">
         <v>800</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>1101</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1231,45 +1278,48 @@
       <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
         <v>10</v>
       </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
-        <v>1</v>
-      </c>
-      <c r="L15" s="4">
-        <v>1</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0</v>
-      </c>
-      <c r="N15" s="8">
-        <v>100110</v>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
       </c>
       <c r="O15" s="5">
+        <v>1001100</v>
+      </c>
+      <c r="P15" s="4">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>1110</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1278,45 +1328,48 @@
       <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5">
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="4">
         <v>10</v>
       </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>1</v>
-      </c>
-      <c r="L16" s="4">
-        <v>1</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0</v>
-      </c>
-      <c r="N16" s="8">
-        <v>1100100110</v>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0</v>
       </c>
       <c r="O16" s="5">
+        <v>11001001100</v>
+      </c>
+      <c r="P16" s="4">
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>1111</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1325,40 +1378,43 @@
       <c r="C17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>1</v>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
       </c>
       <c r="J17" s="4">
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
-        <v>1</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-      <c r="N17" s="8">
-        <v>1000000010010</v>
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0</v>
       </c>
       <c r="O17" s="5">
+        <v>10000000100100</v>
+      </c>
+      <c r="P17" s="4">
         <v>1012</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working Version 6, bneq bug fixed
</commit_message>
<xml_diff>
--- a/control_codes.xlsx
+++ b/control_codes.xlsx
@@ -549,7 +549,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="3">
         <v>0</v>
@@ -1112,10 +1112,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="5">
-        <v>10000001100000</v>
+        <v>10010001100000</v>
       </c>
       <c r="P11" s="4">
-        <v>2060</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>